<commit_message>
ID: OMS-RTM-01-->Update RTM approved
</commit_message>
<xml_diff>
--- a/PM/OnlineMobileStore_RTM.xlsx
+++ b/PM/OnlineMobileStore_RTM.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EAC6BC-C4A0-41A3-8A65-DB1887D73C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Requirements Traceability Matrix (RTM)</t>
   </si>
@@ -55,22 +46,22 @@
     <t>OMS_SRS_Log_01 &amp;  OMS_SRS_Log_02</t>
   </si>
   <si>
-    <t>OMS_SIQ_admin_01 &amp; OMS_CUST_client_07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OMS_SRS_Adm_UD_01 &amp; OMS_SRS_Adm_UD_02 </t>
+    <t>OMS_SIQ_admin_01 &amp; OMS_SIQ_admin_02 &amp;  OMS_CUST_client_07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OMS_SRS_AdmP_01&amp; OMS_SRS_AdmP_02  &amp; OMS_SRS_AdmP_03 &amp; OMS_SRS_AdmP_04 </t>
   </si>
   <si>
     <t>OMS_SIQ_client_05 &amp; OMS_CUST_client_07</t>
   </si>
   <si>
-    <t>OMS_SRS_ Adm_ItD_01 &amp; OMS_SRS_ Adm_ItD_02 &amp; OMS_SRS_Core-B_03</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> OMS_SIQ_hist_11   &amp;  OMS_CUST_client_03</t>
-  </si>
-  <si>
-    <t>OMS_SRS_ Hist_01</t>
+    <t xml:space="preserve"> OMS_SRS_Core-B_03 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OMS_SIQ_hist_10 &amp; OMS_SIQ_hist_11   &amp;  OMS_CUST_client_03</t>
+  </si>
+  <si>
+    <t>OMS_SRS_ Hist_01 &amp; OMS_SRS_ Hist_02</t>
   </si>
   <si>
     <t>OMS_SIQ_client_07</t>
@@ -91,58 +82,68 @@
     <t>OMS_SRS_Core-B_02</t>
   </si>
   <si>
+    <t>OMS_SIQ_client_08</t>
+  </si>
+  <si>
     <t>OMS_SRS_Core-B_05</t>
   </si>
   <si>
-    <t>OMS_SIQ_client_08</t>
-  </si>
-  <si>
-    <t>OMS_SRS_Core-B_06</t>
-  </si>
-  <si>
     <t>OMS_SIQ_client_09</t>
   </si>
   <si>
     <t>OMS_SRS_Core-B_07.01 &amp; OMS_SRS_Core-B_07.02 &amp; OMS_SRS_Core-B_07.03</t>
+  </si>
+  <si>
+    <t>OMS_CUST_client_01 &amp; OMS_CUST_client_02 &amp; OMS_CUST_client_03 &amp; OMS_CUST_client_04 &amp; OMS_CUST_client_05  &amp;  OMS_CUST_client_06 &amp; OMS_CUST_client_07 &amp;OMS_CUST_client_08</t>
+  </si>
+  <si>
+    <t>OMS_SRS_Core-B_08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="7">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
+      <sz val="20.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font/>
+    <font>
+      <sz val="14.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -156,70 +157,98 @@
         <bgColor rgb="FFC8C8C8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
+    <border/>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
-      <diagonal/>
+    </border>
+    <border>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
-      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="medium">
@@ -231,10 +260,6 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -246,10 +271,6 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -261,125 +282,97 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="27">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="8" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="8" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="9" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -569,374 +562,336 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:H1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="8" width="8.6640625" customWidth="1"/>
-    <col min="9" max="9" width="23.6640625" customWidth="1"/>
-    <col min="10" max="26" width="8.6640625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="26.0"/>
+    <col customWidth="1" min="2" max="2" width="26.43"/>
+    <col customWidth="1" min="3" max="3" width="10.29"/>
+    <col customWidth="1" min="4" max="4" width="8.71"/>
+    <col customWidth="1" min="5" max="5" width="12.29"/>
+    <col customWidth="1" min="6" max="8" width="8.71"/>
+    <col customWidth="1" min="9" max="9" width="23.71"/>
+    <col customWidth="1" min="10" max="25" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="37.5" customHeight="1">
-      <c r="A1" s="15" t="s">
+    <row r="1" ht="37.5" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="36" customHeight="1">
-      <c r="A2" s="18" t="s">
+    <row r="2" ht="36.0" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:26" ht="26.25" customHeight="1">
-      <c r="A3" s="1" t="s">
+    <row r="3" ht="26.25" customHeight="1">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
     </row>
-    <row r="4" spans="1:26" ht="124.5" customHeight="1">
-      <c r="A4" s="6" t="s">
+    <row r="4" ht="124.5" customHeight="1">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="91.5" customHeight="1">
-      <c r="A5" s="6" t="s">
+    <row r="5" ht="91.5" customHeight="1">
+      <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="33.75" customHeight="1">
-      <c r="A6" s="6" t="s">
+    <row r="6" ht="70.5" customHeight="1">
+      <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:26" ht="57.75" customHeight="1">
-      <c r="A7" s="6" t="s">
+    <row r="7" ht="57.75" customHeight="1">
+      <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:26" ht="26.25" customHeight="1">
-      <c r="A8" s="6" t="s">
+    <row r="8" ht="52.5" customHeight="1">
+      <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="11" t="s">
+    <row r="9" ht="20.25" customHeight="1">
+      <c r="A9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="11" t="s">
+    <row r="10" ht="24.75" customHeight="1">
+      <c r="A10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="11" t="s">
+    <row r="11" ht="21.0" customHeight="1">
+      <c r="A11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="8" t="s">
+    <row r="12" ht="19.5" customHeight="1">
+      <c r="A12" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="9"/>
+      <c r="B12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="8" t="s">
+    <row r="13" ht="51.0" customHeight="1">
+      <c r="A13" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
+      <c r="B13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
     </row>
-    <row r="14" spans="1:26" ht="51" customHeight="1">
-      <c r="A14" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="7" t="s">
+    <row r="14" ht="111.0" customHeight="1">
+      <c r="A14" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="14"/>
+      <c r="B14" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+      <c r="V14" s="18"/>
+      <c r="W14" s="18"/>
+      <c r="X14" s="18"/>
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="18"/>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="10"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="10"/>
-      <c r="Y15" s="10"/>
-      <c r="Z15" s="10"/>
+    <row r="15" ht="14.25" customHeight="1">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="18"/>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
+    <row r="16" ht="14.25" customHeight="1">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="18"/>
+      <c r="T16" s="18"/>
+      <c r="U16" s="18"/>
+      <c r="V16" s="18"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="18"/>
     </row>
-    <row r="17" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="10"/>
-    </row>
-    <row r="18" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="10"/>
-    </row>
-    <row r="19" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" ht="14.25" customHeight="1"/>
+    <row r="18" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1123,8 +1078,8 @@
     <row r="216" ht="14.25" customHeight="1"/>
     <row r="217" ht="14.25" customHeight="1"/>
     <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
     <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>
     <row r="223" ht="15.75" customHeight="1"/>
@@ -1903,14 +1858,14 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ID: OMS-RTM-02-->update RTM with new doc in sprint
Keep tracking each Module in LLD at RTM and the main doc which gathers all modules.
</commit_message>
<xml_diff>
--- a/PM/OnlineMobileStore_RTM.xlsx
+++ b/PM/OnlineMobileStore_RTM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Requirements Traceability Matrix (RTM)</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">OMS_SRS_Reg_01 &amp; OMS_SRS_Reg_02 &amp;  OMS_SRS_Reg_03 &amp; OMS_SRS_Reg_04 &amp; OMS_SRS_Reg_05 &amp;  OMS_SRS_Reg_06 &amp; OMS_SRS_Reg_07 &amp; OMS_SRS_Reg_08 </t>
   </si>
   <si>
+    <t>OMS-DESIGN-Log&amp;Reg</t>
+  </si>
+  <si>
     <t>OMS_CUST_client_02 &amp; OMS_SIQ_Log_12 &amp;  OMS_SIQ_Log_13 &amp;  OMS_SIQ_Log_15 &amp; OMS_SIQ_Log_16 &amp; OMS_SIQ_Log_17</t>
   </si>
   <si>
@@ -52,12 +55,20 @@
     <t xml:space="preserve">OMS_SRS_AdmP_01&amp; OMS_SRS_AdmP_02  &amp; OMS_SRS_AdmP_03 &amp; OMS_SRS_AdmP_04 </t>
   </si>
   <si>
+    <t xml:space="preserve"> OMS-DESIGN-Pan&amp;Dash
+</t>
+  </si>
+  <si>
     <t>OMS_SIQ_client_05 &amp; OMS_CUST_client_07</t>
   </si>
   <si>
     <t xml:space="preserve"> OMS_SRS_Core-B_03 </t>
   </si>
   <si>
+    <t xml:space="preserve"> OMS-DESIGN-CliBash
+</t>
+  </si>
+  <si>
     <t xml:space="preserve"> OMS_SIQ_hist_10 &amp; OMS_SIQ_hist_11   &amp;  OMS_CUST_client_03</t>
   </si>
   <si>
@@ -67,7 +78,7 @@
     <t>OMS_SIQ_client_07</t>
   </si>
   <si>
-    <t>OMS_SRS_Core-B_01.1</t>
+    <t>OMS_SRS_Core-B_01.1 &amp;OMS_SRS_Core-B_01.3</t>
   </si>
   <si>
     <t>OMS_SIQ_client_03</t>
@@ -76,6 +87,9 @@
     <t>OMS_SRS_Core-B_01.2</t>
   </si>
   <si>
+    <t>OMS-DESIGN-Pan&amp;Dash</t>
+  </si>
+  <si>
     <t>OMS_SIQ_client_04</t>
   </si>
   <si>
@@ -94,10 +108,16 @@
     <t>OMS_SRS_Core-B_07.01 &amp; OMS_SRS_Core-B_07.02 &amp; OMS_SRS_Core-B_07.03</t>
   </si>
   <si>
+    <t xml:space="preserve"> OMS-DESIGN-CliBash   &amp;     OMS-DESIGN-Pan&amp;Dash</t>
+  </si>
+  <si>
     <t>OMS_CUST_client_01 &amp; OMS_CUST_client_02 &amp; OMS_CUST_client_03 &amp; OMS_CUST_client_04 &amp; OMS_CUST_client_05  &amp;  OMS_CUST_client_06 &amp; OMS_CUST_client_07 &amp;OMS_CUST_client_08</t>
   </si>
   <si>
     <t>OMS_SRS_Core-B_08</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OMS-DESIGN-CliBash &amp;     OMS-DESIGN-Pan&amp;Dash  &amp;    OMS-DESIGN-Log&amp;Reg</t>
   </si>
 </sst>
 </file>
@@ -164,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border/>
     <border>
       <left style="medium">
@@ -182,9 +202,7 @@
       <bottom/>
     </border>
     <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -202,9 +220,7 @@
       <bottom/>
     </border>
     <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
     </border>
@@ -237,18 +253,10 @@
       </bottom>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
     </border>
     <border>
       <left style="medium">
@@ -272,22 +280,11 @@
         <color rgb="FF000000"/>
       </top>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -310,9 +307,6 @@
     <xf borderId="8" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -325,39 +319,33 @@
     <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf borderId="9" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,12 +565,12 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="26.0"/>
     <col customWidth="1" min="2" max="2" width="26.43"/>
-    <col customWidth="1" min="3" max="3" width="10.29"/>
+    <col customWidth="1" min="3" max="3" width="30.86"/>
     <col customWidth="1" min="4" max="4" width="8.71"/>
     <col customWidth="1" min="5" max="5" width="12.29"/>
-    <col customWidth="1" min="6" max="8" width="8.71"/>
-    <col customWidth="1" min="9" max="9" width="23.71"/>
-    <col customWidth="1" min="10" max="25" width="8.71"/>
+    <col customWidth="1" min="6" max="6" width="8.71"/>
+    <col customWidth="1" min="7" max="7" width="23.71"/>
+    <col customWidth="1" min="8" max="23" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="37.5" customHeight="1">
@@ -593,9 +581,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" ht="36.0" customHeight="1">
       <c r="A2" s="4" t="s">
@@ -605,9 +591,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" ht="26.25" customHeight="1">
       <c r="A3" s="7" t="s">
@@ -626,255 +610,249 @@
         <v>6</v>
       </c>
       <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
     </row>
     <row r="4" ht="124.5" customHeight="1">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="15"/>
+      <c r="C4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" ht="91.5" customHeight="1">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="15"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" ht="70.5" customHeight="1">
-      <c r="A6" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="17" t="s">
+      <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="B6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="18"/>
     </row>
     <row r="7" ht="57.75" customHeight="1">
-      <c r="A7" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15"/>
+      <c r="A7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" ht="52.5" customHeight="1">
-      <c r="A8" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
+      <c r="A8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
-    <row r="9" ht="20.25" customHeight="1">
-      <c r="A9" s="20" t="s">
+    <row r="9" ht="52.5" customHeight="1">
+      <c r="A9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" ht="24.75" customHeight="1">
-      <c r="A10" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
+      <c r="A10" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" ht="21.0" customHeight="1">
-      <c r="A11" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
+      <c r="A11" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" ht="19.5" customHeight="1">
-      <c r="A12" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="14" t="s">
+      <c r="A12" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
     </row>
-    <row r="13" ht="51.0" customHeight="1">
-      <c r="A13" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="24"/>
+    <row r="13" ht="67.5" customHeight="1">
+      <c r="A13" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
     </row>
-    <row r="14" ht="111.0" customHeight="1">
-      <c r="A14" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
+    <row r="14" ht="153.0" customHeight="1">
+      <c r="A14" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="18"/>
-      <c r="Z15" s="18"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="18"/>
-      <c r="Z16" s="18"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
     </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -1858,10 +1836,12 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
ID:OMS-RTM-03-->update RTM in sprint 4
add code implement and update LLD and HLD comment from sprint 3 "add IDs and some comment on design"
</commit_message>
<xml_diff>
--- a/PM/OnlineMobileStore_RTM.xlsx
+++ b/PM/OnlineMobileStore_RTM.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Requirements Traceability Matrix (RTM)</t>
   </si>
@@ -40,8 +56,10 @@
     <t xml:space="preserve">OMS_SRS_Reg_01 &amp; OMS_SRS_Reg_02 &amp;  OMS_SRS_Reg_03 &amp; OMS_SRS_Reg_04 &amp; OMS_SRS_Reg_05 &amp;  OMS_SRS_Reg_06 &amp; OMS_SRS_Reg_07 &amp; OMS_SRS_Reg_08 </t>
   </si>
   <si>
-    <t>OMS-DESIGN-ERD &amp; 
-DESIGN-UseCase&amp; OMS-DESIGN-Log&amp;Reg</t>
+    <t>OMS-DESIGN-ERD  &amp; OMS-DESIGN-USCSE &amp;  OMS-DESIGN-HLD &amp; OMS-DESIGN-VALREG &amp; OMS-DESIGN-JOIN</t>
+  </si>
+  <si>
+    <t>SignUp.cs  &amp; SignUp.resx</t>
   </si>
   <si>
     <t>OMS_CUST_client_02 &amp; OMS_SIQ_Log_12 &amp;  OMS_SIQ_Log_13 &amp;  OMS_SIQ_Log_15 &amp; OMS_SIQ_Log_16 &amp; OMS_SIQ_Log_17</t>
@@ -50,7 +68,10 @@
     <t>OMS_SRS_Log_01 &amp;  OMS_SRS_Log_02</t>
   </si>
   <si>
-    <t>OMS-DESIGN-ERD  &amp; DESIGN-UseCase &amp; OMS-DESIGN-Log&amp;Reg</t>
+    <t>OMS-DESIGN-ERD  &amp; OMS-DESIGN-USCSE &amp;  OMS-DESIGN-HLD &amp; OMS-DESIGN-VALOG &amp; OMS-DESIGN-CHKLOG</t>
+  </si>
+  <si>
+    <t>LogIn.cs  &amp; LogIn.resx</t>
   </si>
   <si>
     <t>OMS_SIQ_admin_01 &amp; OMS_SIQ_admin_02 &amp;  OMS_CUST_client_07</t>
@@ -59,123 +80,292 @@
     <t xml:space="preserve">OMS_SRS_AdmP_01&amp; OMS_SRS_AdmP_02  &amp; OMS_SRS_AdmP_03 &amp; OMS_SRS_AdmP_04 </t>
   </si>
   <si>
-    <t xml:space="preserve"> OMS-DESIGN-ERD  &amp; DESIGN-UseCase &amp; OMS-DESIGN-Pan&amp;Dash
+    <t>OMS-DESIGN-ERD  &amp; OMS-DESIGN-USCSE &amp;  OMS-DESIGN-HLD &amp; OMS-DESIGN-EXUSR &amp; OMS-DESIGN-EXITM &amp;  OMS-DESIGN-DLUSR &amp; OMS-DESIGN-DLITM    &amp;              OMS-DESIGN-DEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin.Designer.cs  &amp;  Admin.resx  &amp; Form1.Designer.cs   &amp;  Form1.resx &amp;   DeleteProducts.cs &amp; DeleteProducts.resx
+ </t>
+  </si>
+  <si>
+    <t>OMS_SIQ_client_05 &amp; OMS_CUST_client_07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OMS_SRS_Core-B_03 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OMS-DESIGN-ERD  &amp; OMS-DESIGN-USCSE &amp;  OMS-DESIGN-HLD &amp; OMS-DESIGN-SEQ  &amp;  OMS-DESIGN-UPQTY &amp;  OMS-DESIGN-RMCRD   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OMS_SIQ_hist_10 &amp; OMS_SIQ_hist_11   &amp;  OMS_CUST_client_03</t>
+  </si>
+  <si>
+    <t>OMS_SRS_ Hist_01 &amp; OMS_SRS_ Hist_02</t>
+  </si>
+  <si>
+    <t>OMS-DESIGN-ERD  &amp; OMS-DESIGN-USCSE &amp;  OMS-DESIGN-HLD &amp;  OMS-DESIGN-SEQ</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_client_07</t>
+  </si>
+  <si>
+    <t>OMS_SRS_Core-B_01.1 &amp;OMS_SRS_Core-B_01.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OMS-DESIGN-ERD  &amp; OMS-DESIGN-USCSE &amp;  OMS-DESIGN-HLD &amp; OMS-DESIGN-SEQ &amp;  OMS-DESIGN-ADDB &amp; OMS-DESIGN-OUT      
 </t>
   </si>
   <si>
-    <t>OMS_SIQ_client_05 &amp; OMS_CUST_client_07</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> OMS_SRS_Core-B_03 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OMS-DESIGN-ERD  &amp; DESIGN-UseCase &amp;  OMS-DESIGN-CliBash
+    <t>OMS_SIQ_client_03</t>
+  </si>
+  <si>
+    <t>OMS_SRS_Core-B_01.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OMS-DESIGN-ERD  &amp; OMS-DESIGN-USCSE &amp;  OMS-DESIGN-HLD &amp;OMS-DESIGN-SEQ       </t>
+  </si>
+  <si>
+    <t>OMS_SIQ_client_04</t>
+  </si>
+  <si>
+    <t>OMS_SRS_Core-B_02</t>
+  </si>
+  <si>
+    <t>OMS-DESIGN-ERD  &amp; OMS-DESIGN-USCSE &amp;  OMS-DESIGN-HLD &amp; OMS-DESIGN-SEQ</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_client_08</t>
+  </si>
+  <si>
+    <t>OMS_SRS_Core-B_05</t>
+  </si>
+  <si>
+    <t>OMS-DESIGN-ERD  &amp; OMS-DESIGN-USCSE &amp;  OMS-DESIGN-HLD  &amp; OMS-DESIGN-SEQ</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_client_09</t>
+  </si>
+  <si>
+    <t>OMS_SRS_Core-B_07.01 &amp; OMS_SRS_Core-B_07.02 &amp; OMS_SRS_Core-B_07.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OMS-DESIGN-ERD  &amp; OMS-DESIGN-USCSE &amp;  OMS-DESIGN-HLD &amp; OMS-DESIGN-SEQ &amp; OMS-DESIGN-ADCRD &amp;  OMS-DESIGN-RMCRD &amp;  OMS-DESIGN-CNFRM </t>
+  </si>
+  <si>
+    <t>OMS_CUST_client_01 &amp; OMS_CUST_client_02 &amp; OMS_CUST_client_03 &amp; OMS_CUST_client_04 &amp; OMS_CUST_client_05  &amp;  OMS_CUST_client_06 &amp; OMS_CUST_client_07 &amp;OMS_CUST_client_08</t>
+  </si>
+  <si>
+    <t>OMS_SRS_Core-B_08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OMS-DESIGN-ERD  &amp; OMS-DESIGN-USCSE &amp;  OMS-DESIGN-HLD &amp; &amp; OMS-DESIGN-SEQ &amp; OMS-DESIGN-VALREG &amp; OMS-DESIGN-JOIN  &amp; OMS-DESIGN-SEQ &amp;  OMS-DESIGN-ADDB &amp; OMS-DESIGN-OUT   &amp; OMS-DESIGN-SEQ  &amp;  OMS-DESIGN-UPQTY &amp;  OMS-DESIGN-RMCRD  &amp; OMS-DESIGN-EXUSR &amp; OMS-DESIGN-EXITM &amp;  OMS-DESIGN-DLUSR &amp; OMS-DESIGN-DLITM   &amp; OMS-DESIGN-VALOG &amp; OMS-DESIGN-CHKLOG  &amp; OMS-DESIGN-ADCRD &amp;  OMS-DESIGN-RMCRD &amp;  OMS-DESIGN-CNFRM 
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> OMS_SIQ_hist_10 &amp; OMS_SIQ_hist_11   &amp;  OMS_CUST_client_03</t>
-  </si>
-  <si>
-    <t>OMS_SRS_ Hist_01 &amp; OMS_SRS_ Hist_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OMS-DESIGN-ERD  &amp;  DESIGN-UseCase &amp; OMS-DESIGN-CliBash
-</t>
-  </si>
-  <si>
-    <t>OMS_SIQ_client_07</t>
-  </si>
-  <si>
-    <t>OMS_SRS_Core-B_01.1 &amp; OMS_SRS_Core-B_01.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> OMS-DESIGN-ERD  &amp; DESIGN-UseCase &amp; OMS-DESIGN-CliBash
-</t>
-  </si>
-  <si>
-    <t>OMS_SIQ_client_03</t>
-  </si>
-  <si>
-    <t>OMS_SRS_Core-B_01.2</t>
-  </si>
-  <si>
-    <t>OMS-DESIGN-ERD  &amp; DESIGN-UseCase &amp; OMS-DESIGN-Pan&amp;Dash</t>
-  </si>
-  <si>
-    <t>OMS_SIQ_client_04</t>
-  </si>
-  <si>
-    <t>OMS_SRS_Core-B_02</t>
-  </si>
-  <si>
-    <t>OMS_SIQ_client_08</t>
-  </si>
-  <si>
-    <t>OMS_SRS_Core-B_05</t>
-  </si>
-  <si>
-    <t>OMS_SIQ_client_09</t>
-  </si>
-  <si>
-    <t>OMS_SRS_Core-B_07.01 &amp; OMS_SRS_Core-B_07.02 &amp; OMS_SRS_Core-B_07.03</t>
-  </si>
-  <si>
-    <t>OMS-DESIGN-ERD  &amp; DESIGN-UseCase &amp;  OMS-DESIGN-CliBash   &amp;     OMS-DESIGN-Pan&amp;Dash</t>
-  </si>
-  <si>
-    <t>OMS_CUST_client_01 &amp; OMS_CUST_client_02 &amp; OMS_CUST_client_03 &amp; OMS_CUST_client_04 &amp; OMS_CUST_client_05  &amp;  OMS_CUST_client_06 &amp; OMS_CUST_client_07 &amp;OMS_CUST_client_08</t>
-  </si>
-  <si>
-    <t>OMS_SRS_Core-B_08</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DESIGN-UseCase &amp; OMS-DESIGN-CliBash &amp;     OMS-DESIGN-Pan&amp;Dash  &amp;    OMS-DESIGN-Log&amp;Reg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="26">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20.0"/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
     </font>
-    <font/>
     <font>
-      <sz val="14.0"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -195,46 +385,229 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
-    <border/>
+  <borders count="16">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
       <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -249,6 +622,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -263,12 +637,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -280,6 +649,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -291,91 +662,591 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="8" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="8" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="9" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <horizontal style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+    </tableStyle>
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -565,30 +1436,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.0"/>
-    <col customWidth="1" min="2" max="2" width="29.0"/>
-    <col customWidth="1" min="3" max="3" width="27.86"/>
-    <col customWidth="1" min="4" max="4" width="8.71"/>
-    <col customWidth="1" min="5" max="5" width="12.29"/>
-    <col customWidth="1" min="6" max="6" width="8.71"/>
-    <col customWidth="1" min="7" max="7" width="23.71"/>
-    <col customWidth="1" min="8" max="23" width="8.71"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="26.4259259259259" customWidth="1"/>
+    <col min="3" max="3" width="30.8611111111111" customWidth="1"/>
+    <col min="4" max="4" width="35" customWidth="1"/>
+    <col min="5" max="5" width="12.287037037037" customWidth="1"/>
+    <col min="6" max="6" width="8.71296296296296" customWidth="1"/>
+    <col min="7" max="7" width="23.712962962963" customWidth="1"/>
+    <col min="8" max="23" width="8.71296296296296" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="37.5" customHeight="1">
+    <row r="1" ht="37.5" customHeight="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -596,278 +1469,284 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
+      <c r="F1" s="2"/>
     </row>
-    <row r="2" ht="36.0" customHeight="1">
-      <c r="A2" s="4" t="s">
+    <row r="2" ht="36" customHeight="1" spans="1:6">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
-    <row r="3" ht="26.25" customHeight="1">
-      <c r="A3" s="7" t="s">
+    <row r="3" ht="26.25" customHeight="1" spans="1:24">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
     </row>
-    <row r="4" ht="124.5" customHeight="1">
-      <c r="A4" s="11" t="s">
+    <row r="4" ht="124.5" customHeight="1" spans="1:6">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="D4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
-    <row r="5" ht="91.5" customHeight="1">
-      <c r="A5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="12" t="s">
+    <row r="5" ht="91.5" customHeight="1" spans="1:6">
+      <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="C5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
-    <row r="6" ht="70.5" customHeight="1">
-      <c r="A6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="13" t="s">
+    <row r="6" ht="119.25" customHeight="1" spans="1:7">
+      <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
+      <c r="B6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
     </row>
-    <row r="7" ht="57.75" customHeight="1">
-      <c r="A7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+    <row r="7" ht="117" customHeight="1" spans="1:6">
+      <c r="A7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
-    <row r="8" ht="52.5" customHeight="1">
-      <c r="A8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+    <row r="8" ht="73.5" customHeight="1" spans="1:6">
+      <c r="A8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
-    <row r="9" ht="55.5" customHeight="1">
-      <c r="A9" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+    <row r="9" ht="90.75" customHeight="1" spans="1:6">
+      <c r="A9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
-    <row r="10" ht="54.75" customHeight="1">
-      <c r="A10" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+    <row r="10" ht="75" customHeight="1" spans="1:6">
+      <c r="A10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
-    <row r="11" ht="51.0" customHeight="1">
-      <c r="A11" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+    <row r="11" ht="56.25" customHeight="1" spans="1:6">
+      <c r="A11" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
-    <row r="12" ht="44.25" customHeight="1">
-      <c r="A12" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+    <row r="12" ht="54" customHeight="1" spans="1:6">
+      <c r="A12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
-    <row r="13" ht="72.0" customHeight="1">
-      <c r="A13" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
+    <row r="13" ht="111.75" customHeight="1" spans="1:6">
+      <c r="A13" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
     </row>
-    <row r="14" ht="153.0" customHeight="1">
-      <c r="A14" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
+    <row r="14" ht="306.75" customHeight="1" spans="1:24">
+      <c r="A14" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
+    <row r="15" ht="14.25" customHeight="1" spans="1:24">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
+    <row r="16" ht="14.25" customHeight="1" spans="1:24">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
     </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -1858,9 +2737,8 @@
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>